<commit_message>
added tas diagram classification for melt composition matching
</commit_message>
<xml_diff>
--- a/pide/pide_src/eos/Average_Composition_GEOROC.xlsx
+++ b/pide/pide_src/eos/Average_Composition_GEOROC.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="32">
   <si>
     <t xml:space="preserve">Alkali-Basalt</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t xml:space="preserve">FE2O3(WT%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrachyBasalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrachyDacite</t>
   </si>
 </sst>
 </file>
@@ -221,13 +227,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I77" activeCellId="0" sqref="I77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2311,6 +2317,284 @@
       </c>
       <c r="N74" s="2" t="n">
         <f aca="false">SUM(A74:M74)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K77" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L77" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M77" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>49.1599928240624</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>2.00135221435978</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>16.1793838780455</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>0.0354620706087903</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>9.85323331702572</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>8.4665174809513</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>5.48044428322085</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <v>0.173956647485043</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>0.0120906638116253</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <v>2.45386227940377</v>
+      </c>
+      <c r="K78" s="0" t="n">
+        <v>3.65144520286169</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <v>0.654495412723449</v>
+      </c>
+      <c r="M78" s="0" t="n">
+        <v>1.15671641791045</v>
+      </c>
+      <c r="N78" s="2" t="n">
+        <f aca="false">SUM(A78:M78)</f>
+        <v>99.2789526924704</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>50.1007668501417</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>2.03965206088426</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>16.4890084983115</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>0.0361407077082532</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>10.0417944913679</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>8.62854109568068</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>5.5853234611223</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <v>0.177285653170692</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <v>0.0123220426589075</v>
+      </c>
+      <c r="J79" s="0" t="n">
+        <v>2.50082180407866</v>
+      </c>
+      <c r="K79" s="0" t="n">
+        <v>3.72132285351144</v>
+      </c>
+      <c r="L79" s="0" t="n">
+        <v>0.667020481363753</v>
+      </c>
+      <c r="M79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" s="2" t="n">
+        <f aca="false">SUM(A79:M79)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K82" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="L82" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M82" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N82" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>65.1370418540092</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>0.736724639642887</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>15.8511239820027</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>0.00405695561269142</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>4.09043837352238</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>2.7907539381042</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>1.15751397097257</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>0.0952083098759671</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="J83" s="0" t="n">
+        <v>4.27234897751844</v>
+      </c>
+      <c r="K83" s="0" t="n">
+        <v>4.20337982066165</v>
+      </c>
+      <c r="L83" s="0" t="n">
+        <v>0.22801308622974</v>
+      </c>
+      <c r="M83" s="0" t="n">
+        <v>0.551666666666667</v>
+      </c>
+      <c r="N83" s="2" t="n">
+        <f aca="false">SUM(A83:M83)</f>
+        <v>99.1202705748191</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>66.0829506266567</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>0.747423226496519</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>16.0813112426478</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>0.00411587001523502</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>4.1498390068849</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>2.83128078054617</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>1.17432318717952</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>0.0965909083633603</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>0.00202904365152988</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <v>4.33439128497698</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <v>4.26442057004116</v>
+      </c>
+      <c r="L84" s="0" t="n">
+        <v>0.231324252540095</v>
+      </c>
+      <c r="M84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" s="2" t="n">
+        <f aca="false">SUM(A84:M84)</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>